<commit_message>
Extended top banner to right in wireframes
</commit_message>
<xml_diff>
--- a/documentation/MainWindowLayout.xlsx
+++ b/documentation/MainWindowLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\FL22\CSC251 - Adv Java\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\FL22\CSC251 - Adv Java\Group Project\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F6030103-D82F-4438-96F9-BC7A3D60CA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE095CD-8478-4B1B-A749-079AF929AD74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5595BEB3-5ED6-4283-9DE4-821FF5942881}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5595BEB3-5ED6-4283-9DE4-821FF5942881}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>lblAvgMileage</t>
-  </si>
-  <si>
-    <t>lblAverageMPG</t>
   </si>
   <si>
     <t>btnPurchaceVehicle</t>
@@ -254,6 +251,9 @@
       </rPr>
       <t>No Car Selected</t>
     </r>
+  </si>
+  <si>
+    <t>lblAvgMPG</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="58">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -1104,218 +1104,336 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1344,107 +1462,20 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1483,7 +1514,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1092200</xdr:rowOff>
+      <xdr:rowOff>1095375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1549,7 +1580,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1092200</xdr:rowOff>
+      <xdr:rowOff>1095375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1615,7 +1646,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1092200</xdr:rowOff>
+      <xdr:rowOff>1095375</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1967,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED13394E-BB79-4A6C-A436-B357356F716A}">
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L17" sqref="A1:L17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1997,380 +2028,382 @@
   <sheetData>
     <row r="1" spans="1:12" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:12" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="96" t="s">
+      <c r="G2" s="80"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="97"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="99" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="101"/>
-    </row>
-    <row r="3" spans="1:12" s="109" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="108"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="111"/>
-      <c r="K3" s="111"/>
-      <c r="L3" s="111"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="84"/>
+    </row>
+    <row r="3" spans="1:12" s="69" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="2"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
     </row>
     <row r="4" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="62"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="103">
+      <c r="B4" s="47"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="65">
         <v>0</v>
       </c>
-      <c r="E4" s="103">
+      <c r="E4" s="65">
         <v>1</v>
       </c>
-      <c r="F4" s="103">
+      <c r="F4" s="65">
         <v>2</v>
       </c>
-      <c r="G4" s="103">
+      <c r="G4" s="65">
         <v>3</v>
       </c>
-      <c r="H4" s="103">
+      <c r="H4" s="65">
         <v>4</v>
       </c>
-      <c r="I4" s="103">
+      <c r="I4" s="65">
         <v>5</v>
       </c>
-      <c r="J4" s="103">
+      <c r="J4" s="65">
         <v>6</v>
       </c>
-      <c r="K4" s="102"/>
-      <c r="L4" s="56"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="41"/>
     </row>
     <row r="5" spans="1:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="56"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="41"/>
     </row>
     <row r="6" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="63">
+      <c r="B6" s="48">
         <v>0</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="45" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48" t="s">
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="113"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="42"/>
+    </row>
+    <row r="7" spans="1:12" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="48">
+        <v>1</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="42"/>
+    </row>
+    <row r="8" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="48">
+        <v>2</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="57"/>
-    </row>
-    <row r="7" spans="1:12" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="63">
-        <v>1</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="57"/>
-    </row>
-    <row r="8" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="63">
-        <v>2</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="26" t="s">
+      <c r="J8" s="16"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="42"/>
+    </row>
+    <row r="9" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="48">
         <v>3</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="1:12" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="48">
         <v>4</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="48">
+        <v>5</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="57"/>
-    </row>
-    <row r="9" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="63">
-        <v>3</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="88" t="s">
+      <c r="F11" s="86"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="89" t="s">
+      <c r="I11" s="85"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="42"/>
+    </row>
+    <row r="12" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="48">
+        <v>6</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="87"/>
+      <c r="G12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="48">
+        <v>7</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="57"/>
-    </row>
-    <row r="10" spans="1:12" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="63">
-        <v>4</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="57"/>
-    </row>
-    <row r="11" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="63">
-        <v>5</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="104"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="106" t="s">
+      <c r="F13" s="88"/>
+      <c r="G13" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="15"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="48">
+        <v>8</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="49" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="106"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="57"/>
-    </row>
-    <row r="12" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="63">
-        <v>6</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="57"/>
-    </row>
-    <row r="13" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="63">
-        <v>7</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="17"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="57"/>
-    </row>
-    <row r="14" spans="1:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="63">
-        <v>8</v>
-      </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="J14" s="15"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="57"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="63">
+      <c r="B15" s="48">
         <v>9</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="1:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="62"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="56"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="2:23" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="58"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N21" s="5"/>
-      <c r="O21" s="3" t="s">
+      <c r="N21" s="3"/>
+      <c r="O21" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="75"/>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="N22" s="6"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="73"/>
+      <c r="R22" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22" s="74"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N23" s="6"/>
+      <c r="O23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="N22" s="8"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="V22" s="34"/>
-      <c r="W22" s="9"/>
-    </row>
-    <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N23" s="8"/>
-      <c r="O23" s="35" t="s">
+      <c r="P23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="P23" s="36" t="s">
+      <c r="Q23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="37" t="s">
+      <c r="R23" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="37" t="s">
+      <c r="S23" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="S23" s="37" t="s">
+      <c r="T23" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="T23" s="37" t="s">
+      <c r="U23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="U23" s="37" t="s">
+      <c r="V23" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="V23" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="W23" s="9"/>
+      <c r="W23" s="7"/>
     </row>
     <row r="24" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N24" s="8"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="9"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="7"/>
     </row>
     <row r="25" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N25" s="10"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="12"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="I6:J7"/>
     <mergeCell ref="P22:Q22"/>
     <mergeCell ref="R22:T22"/>
     <mergeCell ref="U22:V22"/>
@@ -2385,9 +2418,7 @@
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="E10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2400,7 +2431,7 @@
   <dimension ref="B1:W25"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L17" sqref="A1:L17"/>
+      <selection sqref="A1:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2429,385 +2460,393 @@
   <sheetData>
     <row r="1" spans="2:12" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:12" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="102" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="78"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="108" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="110"/>
     </row>
     <row r="3" spans="2:12" ht="6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="2:12" ht="21.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39">
         <v>0</v>
       </c>
-      <c r="E4" s="54">
+      <c r="E4" s="39">
         <v>1</v>
       </c>
-      <c r="F4" s="54">
+      <c r="F4" s="39">
         <v>2</v>
       </c>
-      <c r="G4" s="54">
+      <c r="G4" s="39">
         <v>3</v>
       </c>
-      <c r="H4" s="54">
+      <c r="H4" s="39">
         <v>4</v>
       </c>
-      <c r="I4" s="54">
+      <c r="I4" s="39">
         <v>5</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="39">
         <v>6</v>
       </c>
-      <c r="K4" s="53"/>
-      <c r="L4" s="55"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="40"/>
     </row>
     <row r="5" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="56"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="41"/>
     </row>
     <row r="6" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="63">
+      <c r="B6" s="48">
         <v>0</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="45" t="s">
+      <c r="C6" s="33"/>
+      <c r="D6" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48" t="s">
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="49" t="s">
+      <c r="I6" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="113"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="42"/>
+    </row>
+    <row r="7" spans="2:12" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="48">
+        <v>1</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="42"/>
+    </row>
+    <row r="8" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="48">
+        <v>2</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="57"/>
-    </row>
-    <row r="7" spans="2:12" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="63">
-        <v>1</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="57"/>
-    </row>
-    <row r="8" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="63">
-        <v>2</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="26" t="s">
+      <c r="J8" s="11"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="42"/>
+    </row>
+    <row r="9" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="48">
         <v>3</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="2:12" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="48">
         <v>4</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="C10" s="32"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="48">
+        <v>5</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="57"/>
-    </row>
-    <row r="9" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="63">
-        <v>3</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="88" t="s">
+      <c r="F11" s="86"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="89" t="s">
+      <c r="I11" s="85"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="42"/>
+    </row>
+    <row r="12" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="48">
+        <v>6</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="87"/>
+      <c r="G12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="48">
+        <v>7</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="57"/>
-    </row>
-    <row r="10" spans="2:12" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="63">
-        <v>4</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="57"/>
-    </row>
-    <row r="11" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="63">
-        <v>5</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="104" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="104"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="106" t="s">
-        <v>6</v>
-      </c>
-      <c r="I11" s="106"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="57"/>
-    </row>
-    <row r="12" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="63">
-        <v>6</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="23" t="s">
+      <c r="F13" s="88"/>
+      <c r="G13" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="57"/>
-    </row>
-    <row r="13" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="63">
-        <v>7</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="30"/>
-      <c r="G13" s="23" t="s">
+      <c r="I13" s="100" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="48">
+        <v>8</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H13" s="23" t="s">
+      <c r="H14" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="101"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="42"/>
+    </row>
+    <row r="15" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="48">
+        <v>9</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="15"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="57"/>
-    </row>
-    <row r="14" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="63">
-        <v>8</v>
-      </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="57"/>
-    </row>
-    <row r="15" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="63">
-        <v>9</v>
-      </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="57"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="62"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="56"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="2:23" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="58"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N21" s="5"/>
-      <c r="O21" s="3" t="s">
+      <c r="N21" s="3"/>
+      <c r="O21" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="75"/>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="N22" s="6"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="73"/>
+      <c r="R22" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22" s="74"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N23" s="6"/>
+      <c r="O23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="N22" s="8"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="V22" s="34"/>
-      <c r="W22" s="9"/>
-    </row>
-    <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N23" s="8"/>
-      <c r="O23" s="35" t="s">
+      <c r="P23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="P23" s="36" t="s">
+      <c r="Q23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="37" t="s">
+      <c r="R23" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="37" t="s">
+      <c r="S23" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="S23" s="37" t="s">
+      <c r="T23" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="T23" s="37" t="s">
+      <c r="U23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="U23" s="37" t="s">
+      <c r="V23" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="V23" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="W23" s="9"/>
+      <c r="W23" s="7"/>
     </row>
     <row r="24" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N24" s="8"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="9"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="7"/>
     </row>
     <row r="25" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N25" s="10"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="12"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G8:G9"/>
     <mergeCell ref="P22:Q22"/>
     <mergeCell ref="R22:T22"/>
     <mergeCell ref="U22:V22"/>
@@ -2818,14 +2857,6 @@
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="O21:V21"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2837,8 +2868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E879955-AA1F-4D95-95E6-FEE76F8284D1}">
   <dimension ref="B1:W25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="A1:L17"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2867,372 +2898,372 @@
   <sheetData>
     <row r="1" spans="2:12" ht="1.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:12" ht="46.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="102" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="74"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="76" t="s">
+      <c r="G2" s="106"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="108" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="110"/>
+    </row>
+    <row r="3" spans="2:12" ht="6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+    </row>
+    <row r="4" spans="2:12" ht="21.5" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39">
+        <v>0</v>
+      </c>
+      <c r="E4" s="39">
+        <v>1</v>
+      </c>
+      <c r="F4" s="39">
+        <v>2</v>
+      </c>
+      <c r="G4" s="39">
+        <v>3</v>
+      </c>
+      <c r="H4" s="39">
+        <v>4</v>
+      </c>
+      <c r="I4" s="39">
+        <v>5</v>
+      </c>
+      <c r="J4" s="39">
+        <v>6</v>
+      </c>
+      <c r="K4" s="38"/>
+      <c r="L4" s="40"/>
+    </row>
+    <row r="5" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="47"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="41"/>
+    </row>
+    <row r="6" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="48">
+        <v>0</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="93" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="111" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="113"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="42"/>
+    </row>
+    <row r="7" spans="2:12" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="48">
+        <v>1</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="114"/>
+      <c r="J7" s="115"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="42"/>
+    </row>
+    <row r="8" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="48">
+        <v>2</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="95" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="11"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="42"/>
+    </row>
+    <row r="9" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="48">
+        <v>3</v>
+      </c>
+      <c r="C9" s="32"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="J2" s="77"/>
-      <c r="K2" s="77"/>
-      <c r="L2" s="78"/>
-    </row>
-    <row r="3" spans="2:12" ht="6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-    </row>
-    <row r="4" spans="2:12" ht="21.5" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54">
-        <v>0</v>
-      </c>
-      <c r="E4" s="54">
-        <v>1</v>
-      </c>
-      <c r="F4" s="54">
-        <v>2</v>
-      </c>
-      <c r="G4" s="54">
-        <v>3</v>
-      </c>
-      <c r="H4" s="54">
+      <c r="I9" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="2:12" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="48">
         <v>4</v>
       </c>
-      <c r="I4" s="54">
+      <c r="C10" s="32"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="97"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="48">
         <v>5</v>
       </c>
-      <c r="J4" s="54">
+      <c r="C11" s="32"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="42"/>
+    </row>
+    <row r="12" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="48">
         <v>6</v>
       </c>
-      <c r="K4" s="53"/>
-      <c r="L4" s="55"/>
-    </row>
-    <row r="5" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="62"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="56"/>
-    </row>
-    <row r="6" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="63">
-        <v>0</v>
-      </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="49" t="s">
+      <c r="C12" s="32"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="48">
+        <v>7</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="48">
         <v>8</v>
       </c>
-      <c r="J6" s="15"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="57"/>
-    </row>
-    <row r="7" spans="2:12" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="63">
-        <v>1</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="57"/>
-    </row>
-    <row r="8" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="63">
-        <v>2</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="27" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" s="24" t="s">
+      <c r="C14" s="32"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="42"/>
+    </row>
+    <row r="15" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="48">
         <v>9</v>
       </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="57"/>
-    </row>
-    <row r="9" spans="2:12" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="63">
-        <v>3</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="88" t="s">
-        <v>5</v>
-      </c>
-      <c r="I9" s="89" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="57"/>
-    </row>
-    <row r="10" spans="2:12" ht="96" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="63">
-        <v>4</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="91"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="91"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="57"/>
-    </row>
-    <row r="11" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="63">
-        <v>5</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="57"/>
-    </row>
-    <row r="12" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="63">
-        <v>6</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="82"/>
-      <c r="H12" s="82"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="57"/>
-    </row>
-    <row r="13" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="63">
-        <v>7</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="83"/>
-      <c r="F13" s="83"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="82"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="57"/>
-    </row>
-    <row r="14" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="63">
-        <v>8</v>
-      </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="82"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="57"/>
-    </row>
-    <row r="15" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="63">
-        <v>9</v>
-      </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="82"/>
-      <c r="H15" s="82"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="57"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="62"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="56"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="2:23" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="59"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="58"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="43"/>
     </row>
     <row r="18" spans="2:23" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="20" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="21" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N21" s="5"/>
-      <c r="O21" s="3" t="s">
+      <c r="N21" s="3"/>
+      <c r="O21" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="P21" s="75"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="75"/>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+      <c r="U21" s="75"/>
+      <c r="V21" s="75"/>
+      <c r="W21" s="4"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="N22" s="6"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q22" s="73"/>
+      <c r="R22" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+      <c r="U22" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="V22" s="74"/>
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="N23" s="6"/>
+      <c r="O23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="3"/>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-      <c r="V21" s="3"/>
-      <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="N22" s="8"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="V22" s="34"/>
-      <c r="W22" s="9"/>
-    </row>
-    <row r="23" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N23" s="8"/>
-      <c r="O23" s="35" t="s">
+      <c r="P23" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="P23" s="36" t="s">
+      <c r="Q23" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q23" s="37" t="s">
+      <c r="R23" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="R23" s="37" t="s">
+      <c r="S23" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="S23" s="37" t="s">
+      <c r="T23" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="T23" s="37" t="s">
+      <c r="U23" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="U23" s="37" t="s">
+      <c r="V23" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="V23" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="W23" s="9"/>
+      <c r="W23" s="7"/>
     </row>
     <row r="24" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N24" s="8"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="40"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="40"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="40"/>
-      <c r="V24" s="41"/>
-      <c r="W24" s="9"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="30"/>
+      <c r="Q24" s="30"/>
+      <c r="R24" s="30"/>
+      <c r="S24" s="30"/>
+      <c r="T24" s="30"/>
+      <c r="U24" s="30"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="7"/>
     </row>
     <row r="25" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="N25" s="10"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="12"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="I6:J7"/>
     <mergeCell ref="O21:V21"/>
     <mergeCell ref="P22:Q22"/>
     <mergeCell ref="R22:T22"/>
     <mergeCell ref="U22:V22"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="E10:I10"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>